<commit_message>
actualizar backlog e HT
</commit_message>
<xml_diff>
--- a/Documentos/Product Backlog.xlsx
+++ b/Documentos/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTOAPPS2\nova\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AD3E8B-481A-4098-9E1C-664A44A6B692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD38AA9-6A45-40F0-89FB-B0F4ECEDBFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="179">
   <si>
     <t>Columna</t>
   </si>
@@ -654,6 +654,18 @@
   </si>
   <si>
     <t>Capa de acceso a datos creada</t>
+  </si>
+  <si>
+    <t>HT-0004</t>
+  </si>
+  <si>
+    <t>Como un desarrollador, necesito elaborar los diagramas de actividades de las funcionalidades del proyecto, con la finalidad de comprender con mayor claridad las condiciones y limitaciones asociadas con cada operación específica.</t>
+  </si>
+  <si>
+    <t>Diagrama de actividades</t>
+  </si>
+  <si>
+    <t>Un diagrama de actividades por cada funcionalidad</t>
   </si>
 </sst>
 </file>
@@ -1090,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I49"/>
+  <dimension ref="B1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1106,7 +1118,7 @@
     <col min="6" max="6" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.77734375" style="2" customWidth="1"/>
     <col min="10" max="10" width="2.109375" style="2" customWidth="1"/>
     <col min="11" max="16384" width="11.44140625" style="2"/>
   </cols>
@@ -1225,30 +1237,30 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>176</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>23</v>
+        <v>177</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>61</v>
+        <v>165</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -1277,21 +1289,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>25</v>
@@ -1300,50 +1312,50 @@
         <v>26</v>
       </c>
       <c r="I10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>37</v>
@@ -1352,24 +1364,24 @@
         <v>26</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>37</v>
@@ -1378,50 +1390,50 @@
         <v>26</v>
       </c>
       <c r="I13" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
+    <row r="15" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="5" t="s">
+      <c r="E15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>50</v>
@@ -1430,24 +1442,24 @@
         <v>26</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>50</v>
@@ -1456,18 +1468,18 @@
         <v>26</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>61</v>
@@ -1476,24 +1488,24 @@
         <v>59</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>99</v>
+      <c r="I17" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>61</v>
@@ -1512,20 +1524,20 @@
       </c>
     </row>
     <row r="19" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>102</v>
+      <c r="B19" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>64</v>
@@ -1539,19 +1551,19 @@
     </row>
     <row r="20" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>64</v>
@@ -1563,24 +1575,24 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>26</v>
@@ -1591,19 +1603,19 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>31</v>
+        <v>110</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>65</v>
@@ -1617,19 +1629,19 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>65</v>
@@ -1643,19 +1655,19 @@
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>65</v>
@@ -1669,13 +1681,13 @@
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>61</v>
@@ -1693,24 +1705,24 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>26</v>
@@ -1721,19 +1733,19 @@
     </row>
     <row r="27" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>66</v>
@@ -1747,13 +1759,13 @@
     </row>
     <row r="28" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>61</v>
@@ -1773,13 +1785,13 @@
     </row>
     <row r="29" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>61</v>
@@ -1799,13 +1811,13 @@
     </row>
     <row r="30" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>82</v>
+        <v>132</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>133</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>63</v>
+        <v>134</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>61</v>
@@ -1814,12 +1826,12 @@
         <v>24</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I30" s="8" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1828,10 +1840,10 @@
         <v>135</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>61</v>
@@ -1854,16 +1866,16 @@
         <v>135</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>64</v>
@@ -1880,10 +1892,10 @@
         <v>135</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>61</v>
@@ -1892,7 +1904,7 @@
         <v>31</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>26</v>
@@ -1903,13 +1915,13 @@
     </row>
     <row r="34" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>61</v>
@@ -1932,19 +1944,19 @@
         <v>136</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>26</v>
@@ -1955,19 +1967,19 @@
     </row>
     <row r="36" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>66</v>
@@ -1984,16 +1996,16 @@
         <v>137</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>66</v>
@@ -2010,16 +2022,16 @@
         <v>137</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>66</v>
@@ -2036,19 +2048,19 @@
         <v>137</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>26</v>
@@ -2059,13 +2071,13 @@
     </row>
     <row r="40" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>61</v>
@@ -2088,10 +2100,10 @@
         <v>138</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>61</v>
@@ -2114,10 +2126,10 @@
         <v>138</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>61</v>
@@ -2140,16 +2152,16 @@
         <v>138</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>61</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>67</v>
@@ -2166,10 +2178,10 @@
         <v>138</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>61</v>
@@ -2187,133 +2199,159 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B46" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D46" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B46" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>142</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>147</v>
+        <v>36</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>142</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>152</v>
+        <v>26</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>142</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>26</v>
+        <v>152</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>142</v>
       </c>
       <c r="F49" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B50" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="G50" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I49" s="5" t="s">
+      <c r="H50" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I50" s="5" t="s">
         <v>161</v>
       </c>
     </row>

</xml_diff>

<commit_message>
historias y documentos actualizados
</commit_message>
<xml_diff>
--- a/Documentos/Product Backlog.xlsx
+++ b/Documentos/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTOAPPS2\nova\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE9A815-5FFB-47CE-B9F0-FAB261F7FF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FF4579-41BC-48D0-BD1C-598DAB3E6DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Historias de Usuario'!$A$1:$I$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$13</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="264">
   <si>
     <t>Columna</t>
   </si>
@@ -119,9 +119,6 @@
     <t>3 puntos</t>
   </si>
   <si>
-    <t>Verificar credenciales</t>
-  </si>
-  <si>
     <t>01-0002-0001</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>Sprint 2</t>
   </si>
   <si>
-    <t>Guardar y actualizar productos</t>
-  </si>
-  <si>
     <t>01-0002-0002</t>
   </si>
   <si>
@@ -149,9 +143,6 @@
     <t>Modificar Producto</t>
   </si>
   <si>
-    <t>Registro de modificaciones</t>
-  </si>
-  <si>
     <t>01-0002-0003</t>
   </si>
   <si>
@@ -161,9 +152,6 @@
     <t>Eliminar Producto</t>
   </si>
   <si>
-    <t>Registro de eliminacion</t>
-  </si>
-  <si>
     <t>01-0003-0001</t>
   </si>
   <si>
@@ -176,9 +164,6 @@
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Navegar, filtrar y ver detalles</t>
-  </si>
-  <si>
     <t>01-0003-0002</t>
   </si>
   <si>
@@ -188,9 +173,6 @@
     <t>Filtrar Productos</t>
   </si>
   <si>
-    <t>Filtros por categoría, precio, características</t>
-  </si>
-  <si>
     <t>01-0003-0003</t>
   </si>
   <si>
@@ -201,9 +183,6 @@
   </si>
   <si>
     <t>4 puntos</t>
-  </si>
-  <si>
-    <t>Nombre, descripción, precio, disponibilidad</t>
   </si>
   <si>
     <t>Planificada</t>
@@ -849,6 +828,99 @@
   </si>
   <si>
     <t>Vista Catalogo productos del Proveedor</t>
+  </si>
+  <si>
+    <t>Como un desarrollador, necesito elaborar el mapa de navegación de mi sistema, con la finalidad de proporcionar la logica de navegcaión que el usuario deberá seguir al momento de usarlo.</t>
+  </si>
+  <si>
+    <t>Mapa de navegación</t>
+  </si>
+  <si>
+    <t>Sprint5</t>
+  </si>
+  <si>
+    <t>HT-0016</t>
+  </si>
+  <si>
+    <t>HT-0017</t>
+  </si>
+  <si>
+    <t>Como un desarrollador, quiero implementar las interfaces de la capa presentación correspondiente a la función "Sistema de Registro y Autenticación"</t>
+  </si>
+  <si>
+    <t>Capa presentación "Sistema de Registro y Autenticación"</t>
+  </si>
+  <si>
+    <t>Iniciada</t>
+  </si>
+  <si>
+    <t>HT-0018</t>
+  </si>
+  <si>
+    <t>Como un desarrollador, quiero implementar las interfaces de la capa presentación correspondiente a la función "Gestión de Inventario"</t>
+  </si>
+  <si>
+    <t>Capa presentación "Sistema de Gestión de Productos"</t>
+  </si>
+  <si>
+    <t>HT-0019</t>
+  </si>
+  <si>
+    <t>Como un desarrollador, quiero implementar las interfaces de la capa presentación correspondiente a la función "Catálogo de Productos"</t>
+  </si>
+  <si>
+    <t>Capa presentación "Catálogo de Productos"</t>
+  </si>
+  <si>
+    <t>HT-0020</t>
+  </si>
+  <si>
+    <t>Como un desarrollador, quiero implementar las interfaces de la capa presentación correspondiente a la función "Asistente Virtual con Inteligencia Artificial"</t>
+  </si>
+  <si>
+    <t>Capa presentación "Asistente Virtual con Inteligencia Artificial"</t>
+  </si>
+  <si>
+    <t>HT-0021</t>
+  </si>
+  <si>
+    <t>Como un desarrollador, quiero implementar las interfaces de la capa presentación correspondiente a la función "Carrito de Compras"</t>
+  </si>
+  <si>
+    <t>Capa presentación "Carrito de Compras"</t>
+  </si>
+  <si>
+    <t>HT-0022</t>
+  </si>
+  <si>
+    <t>Como un desarrollador, quiero implementar las interfaces de la capa presentación correspondiente a la función "Proceso de Pago"</t>
+  </si>
+  <si>
+    <t>Capa presentación "Proceso de Pago"</t>
+  </si>
+  <si>
+    <t>HT-0023</t>
+  </si>
+  <si>
+    <t>Como un desarrollador, quiero implementar las interfaces de la capa presentación correspondiente a la función "Sistema de Gestión de Ventas"</t>
+  </si>
+  <si>
+    <t>Capa presentación "Sistema de Gestión de Ventas"</t>
+  </si>
+  <si>
+    <t>HT-0024</t>
+  </si>
+  <si>
+    <t>Como un desarrollador, quiero implementar las interfaces de la capa presentación correspondiente a la función "Sistema de medición de satisfacción"</t>
+  </si>
+  <si>
+    <t>Capa presentación "Sistema de medición de satisfacción"</t>
+  </si>
+  <si>
+    <t>HT-0025</t>
+  </si>
+  <si>
+    <t>Como un desarrollador, quiero implementar las interfaces de la capa presentación correspondiente a la función "Gestión de Registro de Compras de Productos a los Proveedores"</t>
   </si>
 </sst>
 </file>
@@ -953,7 +1025,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -981,6 +1053,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1285,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I72"/>
+  <dimension ref="B1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="B32" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1313,7 +1388,7 @@
     </row>
     <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1344,16 +1419,16 @@
     </row>
     <row r="5" spans="2:9" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>27</v>
@@ -1365,1715 +1440,1964 @@
         <v>23</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="12" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="5"/>
+      <c r="I12" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="14" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="15" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="16" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="17" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="5"/>
+      <c r="I17" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="18" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="5"/>
+      <c r="I18" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="19" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="20" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="5"/>
+      <c r="I20" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="21" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="5"/>
+      <c r="I21" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="22" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="5"/>
+      <c r="I22" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="23" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="5"/>
+      <c r="I23" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="24" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="5"/>
+      <c r="I24" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="25" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="5"/>
+      <c r="I25" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="26" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="5"/>
+      <c r="I26" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="27" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="H27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="5"/>
+      <c r="I27" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="28" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B29" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F29" s="5" t="s">
+      <c r="H29" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B30" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="H30" s="5" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F31" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="H31" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>25</v>
+        <v>230</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>231</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>26</v>
+        <v>232</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>57</v>
+        <v>154</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I33" s="5" t="s">
-        <v>28</v>
+      <c r="I33" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>30</v>
+        <v>237</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>238</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>31</v>
+        <v>239</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>57</v>
+        <v>240</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I34" s="5" t="s">
-        <v>34</v>
+      <c r="I34" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>36</v>
+        <v>241</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>242</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>37</v>
+        <v>243</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>57</v>
+        <v>240</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="5" t="s">
-        <v>38</v>
+      <c r="I35" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>40</v>
+        <v>244</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>245</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>41</v>
+        <v>246</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>57</v>
+        <v>240</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I36" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>44</v>
+        <v>247</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>248</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>45</v>
+        <v>249</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>57</v>
+        <v>240</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I37" s="5" t="s">
-        <v>47</v>
+      <c r="I37" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="G38" s="5" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I38" s="5" t="s">
-        <v>51</v>
+      <c r="I38" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>53</v>
+        <v>253</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>254</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>54</v>
+        <v>255</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>57</v>
+        <v>240</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="I39" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B40" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="H40" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" ht="105" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>95</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>260</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>96</v>
+        <v>261</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>57</v>
+        <v>240</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>98</v>
+        <v>262</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>263</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>99</v>
+        <v>239</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>57</v>
+        <v>240</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>101</v>
+        <v>24</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>104</v>
+        <v>28</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>108</v>
+        <v>33</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F45" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B46" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I45" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="G46" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>114</v>
+        <v>39</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>117</v>
+        <v>43</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I48" s="8" t="s">
-        <v>90</v>
+      <c r="I48" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>120</v>
+        <v>46</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>121</v>
+        <v>48</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I49" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I49" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>123</v>
+        <v>84</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I50" s="8" t="s">
-        <v>90</v>
+      <c r="I50" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B51" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>126</v>
+      <c r="B51" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I51" s="8" t="s">
-        <v>90</v>
+      <c r="I51" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B52" s="5" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="8" t="s">
-        <v>90</v>
+      <c r="I52" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B53" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>78</v>
+        <v>93</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>65</v>
+        <v>96</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>77</v>
+        <v>100</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>101</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>79</v>
+        <v>103</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>80</v>
+        <v>106</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>81</v>
+        <v>109</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="H58" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B59" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>81</v>
+        <v>112</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B60" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>82</v>
+        <v>115</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H60" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B61" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>83</v>
+        <v>118</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>119</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B62" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>84</v>
+        <v>121</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>122</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>73</v>
+        <v>123</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="63" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B63" s="5" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I63" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I63" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B64" s="5" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I64" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I64" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B65" s="5" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I65" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I65" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B66" s="5" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="H66" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I66" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="67" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I66" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B67" s="5" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G67" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B68" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B69" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H67" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I67" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="68" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B68" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="69" spans="2:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="B69" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="E69" s="5" t="s">
-        <v>138</v>
+        <v>50</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I69" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="70" spans="2:9" ht="86.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B70" s="5" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>147</v>
+        <v>64</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>138</v>
+        <v>50</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H70" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B71" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B72" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B73" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B74" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B75" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B76" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B77" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B78" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B79" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B80" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B81" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B82" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C82" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="I70" s="5" t="s">
+      <c r="D82" s="5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="71" spans="2:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B71" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H71" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" spans="2:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B72" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H72" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I72" s="5" t="s">
-        <v>157</v>
+      <c r="E82" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>